<commit_message>
phys uri labwork airbrushing info
</commit_message>
<xml_diff>
--- a/data/Physiology-URI-labwork.xlsx
+++ b/data/Physiology-URI-labwork.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF941B7-2539-4F46-8C84-5C580C1E9682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415DF285-9AE7-6B4C-9CE2-60FED951642A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="460" windowWidth="28040" windowHeight="19580" xr2:uid="{A8334511-D0E0-DA42-8F89-A6B529CE2D9F}"/>
+    <workbookView xWindow="33600" yWindow="-3080" windowWidth="38400" windowHeight="21140" xr2:uid="{A8334511-D0E0-DA42-8F89-A6B529CE2D9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="28">
   <si>
     <t>ColonyID</t>
   </si>
@@ -92,16 +92,34 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Bag leaked ~4-5 mL spilled out</t>
-  </si>
-  <si>
     <t>2 tubes</t>
   </si>
   <si>
-    <t>3-4 mL spilled out</t>
-  </si>
-  <si>
     <t xml:space="preserve">2 tubes </t>
+  </si>
+  <si>
+    <t>10 + 3-4 mL spilled out</t>
+  </si>
+  <si>
+    <t>7 + Bag leaked ~4-5 mL spilled out</t>
+  </si>
+  <si>
+    <t>tiny</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>no more fragment</t>
+  </si>
+  <si>
+    <t>tiny; no extra homogenate; double the SA for 2 fragments b/c half of skeleton crumbled in bag</t>
+  </si>
+  <si>
+    <t>11 + 1-2 mL leaked out</t>
+  </si>
+  <si>
+    <t>fragment crumbled</t>
   </si>
 </sst>
 </file>
@@ -504,7 +522,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,7 +530,7 @@
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="33" customWidth="1"/>
+    <col min="9" max="9" width="80.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -611,7 +629,9 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
@@ -632,8 +652,12 @@
       <c r="F5" s="5">
         <v>43662</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H5" s="3">
+        <v>8.5</v>
+      </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -655,8 +679,12 @@
       <c r="F6" s="5">
         <v>43662</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H6" s="3">
+        <v>8</v>
+      </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -680,7 +708,9 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
@@ -701,9 +731,15 @@
       <c r="F8" s="5">
         <v>43662</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
@@ -747,9 +783,15 @@
       <c r="F10" s="5">
         <v>43662</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="G10" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
@@ -793,8 +835,12 @@
       <c r="F12" s="5">
         <v>43662</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -816,8 +862,12 @@
       <c r="F13" s="5">
         <v>43662</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="G13" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H13" s="3">
+        <v>7.5</v>
+      </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -839,8 +889,12 @@
       <c r="F14" s="5">
         <v>43662</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4.5</v>
+      </c>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -908,8 +962,12 @@
       <c r="F17" s="5">
         <v>43662</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="G17" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H17" s="3">
+        <v>7</v>
+      </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -931,8 +989,12 @@
       <c r="F18" s="5">
         <v>43662</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="G18" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H18" s="3">
+        <v>7</v>
+      </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -954,9 +1016,15 @@
       <c r="F19" s="5">
         <v>43662</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="G19" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H19" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
@@ -977,8 +1045,12 @@
       <c r="F20" s="5">
         <v>43662</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="G20" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H20" s="3">
+        <v>11.5</v>
+      </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1057,7 +1129,7 @@
         <v>24</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1083,7 +1155,7 @@
         <v>20220321</v>
       </c>
       <c r="H24" s="3">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>20</v>
@@ -1108,9 +1180,15 @@
       <c r="F25" s="5">
         <v>43803</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="G25" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H25" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
@@ -1138,7 +1216,7 @@
         <v>26.5</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1167,7 +1245,7 @@
         <v>28</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1243,8 +1321,12 @@
       <c r="F30" s="5">
         <v>43803</v>
       </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="G30" s="3">
+        <v>20220411</v>
+      </c>
+      <c r="H30" s="3">
+        <v>14</v>
+      </c>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1273,7 +1355,7 @@
         <v>17.5</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1299,10 +1381,10 @@
         <v>20220321</v>
       </c>
       <c r="H32" s="3">
-        <v>7</v>
+        <v>11.5</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1428,9 +1510,15 @@
       <c r="F37" s="5">
         <v>43803</v>
       </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
+      <c r="G37" s="9">
+        <v>20220411</v>
+      </c>
+      <c r="H37" s="3">
+        <v>16</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="4">

</xml_diff>